<commit_message>
update publisher release 54924be1426f52b1cb8f0c303fbd3fbac7f015c9
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-fr-core-appointment.xlsx
+++ b/main/ig/StructureDefinition-fr-core-appointment.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-15T15:07:51+00:00</t>
+    <t>2025-10-22T14:21:04+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -443,7 +443,7 @@
     <t>Appointment.meta.profile</t>
   </si>
   <si>
-    <t xml:space="preserve">canonical(StructureDefinition)
+    <t xml:space="preserve">canonical(StructureDefinition|4.0.1)
 </t>
   </si>
   <si>
@@ -494,7 +494,7 @@
     <t>Security Labels from the Healthcare Privacy and Security Classification System.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/security-labels</t>
+    <t>http://hl7.org/fhir/ValueSet/security-labels|4.0.1</t>
   </si>
   <si>
     <t>Meta.security</t>
@@ -518,7 +518,7 @@
     <t>Codes that represent various types of tags, commonly workflow-related; e.g. "Needs review by Dr. Jones".</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/common-tags</t>
+    <t>http://hl7.org/fhir/ValueSet/common-tags|4.0.1</t>
   </si>
   <si>
     <t>Meta.tag</t>
@@ -561,7 +561,7 @@
     <t>A human language.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/languages</t>
+    <t>http://hl7.org/fhir/ValueSet/languages|4.0.1</t>
   </si>
   <si>
     <t>Resource.language</t>
@@ -746,7 +746,7 @@
     <t>The coded reason for the appointment being cancelled. This is often used in reporting/billing/futher processing to determine if further actions are required, or specific fees apply.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/appointment-cancellation-reason</t>
+    <t>http://hl7.org/fhir/ValueSet/appointment-cancellation-reason|4.0.1</t>
   </si>
   <si>
     <t>Appointment.serviceCategory</t>
@@ -758,7 +758,7 @@
     <t>A broad categorization of the service that is to be performed during this appointment.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/service-category</t>
+    <t>http://hl7.org/fhir/ValueSet/service-category|4.0.1</t>
   </si>
   <si>
     <t>n/a, might be inferred from the ServiceDeliveryLocation</t>
@@ -779,7 +779,7 @@
     <t>For a provider to provider appointment the code "FOLLOWUP" may be appropriate, as this is expected to be discussing some patient that was seen in the past.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/service-type</t>
+    <t>http://hl7.org/fhir/ValueSet/service-type|4.0.1</t>
   </si>
   <si>
     <t>Request.code</t>
@@ -836,7 +836,7 @@
     <t>The Reason for the appointment to take place.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/encounter-reason</t>
+    <t>http://hl7.org/fhir/ValueSet/encounter-reason|4.0.1</t>
   </si>
   <si>
     <t>Request.reasonCode</t>
@@ -851,7 +851,7 @@
     <t>Appointment.reasonReference</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Condition|Procedure|Observation|ImmunizationRecommendation)
+    <t xml:space="preserve">Reference(Condition|4.0.1|Procedure|4.0.1|Observation|4.0.1|ImmunizationRecommendation|4.0.1)
 </t>
   </si>
   <si>
@@ -918,7 +918,7 @@
     <t>Appointment.supportingInformation</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Resource)
+    <t xml:space="preserve">Reference(Resource|4.0.1)
 </t>
   </si>
   <si>
@@ -1087,7 +1087,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(ServiceRequest)
+    <t xml:space="preserve">Reference(ServiceRequest|4.0.1)
 </t>
   </si>
   <si>
@@ -1174,7 +1174,7 @@
     <t>Role of participant in encounter.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/encounter-participant-type</t>
+    <t>http://hl7.org/fhir/ValueSet/encounter-participant-type|4.0.1</t>
   </si>
   <si>
     <t>(performer | reusableDevice | subject | location).@typeCode</t>
@@ -1629,7 +1629,7 @@
     <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="84.54296875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="52.66796875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="53.0859375" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>

</xml_diff>